<commit_message>
rename dataset for same sequence on server
</commit_message>
<xml_diff>
--- a/Datasets/dataset_description.xlsx
+++ b/Datasets/dataset_description.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="28128" windowHeight="12660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -43,6 +43,228 @@
     <t>abalone11–17</t>
   </si>
   <si>
+    <t>abalone19</t>
+  </si>
+  <si>
+    <t>abalone4–8</t>
+  </si>
+  <si>
+    <t>abalone5–10</t>
+  </si>
+  <si>
+    <t>abalone9-18</t>
+  </si>
+  <si>
+    <t>breast</t>
+  </si>
+  <si>
+    <t>cleveland-0_vs_4</t>
+  </si>
+  <si>
+    <t>ecoli-0-1-3-7_vs_2-6</t>
+  </si>
+  <si>
+    <t>ecoli-0-1-4-6_vs_5</t>
+  </si>
+  <si>
+    <t>ecoli-0-1-4-7_vs_2-3-5-6</t>
+  </si>
+  <si>
+    <t>ecoli-0-1-4-7_vs_5-6</t>
+  </si>
+  <si>
+    <t>ecoli-0-1_vs_2-3-5</t>
+  </si>
+  <si>
+    <t>ecoli-0-1_vs_5</t>
+  </si>
+  <si>
+    <t>ecoli-0-2-3-4_vs_5</t>
+  </si>
+  <si>
+    <t>ecoli-0-2-6-7_vs_3-5</t>
+  </si>
+  <si>
+    <t>ecoli-0-3-4-6_vs_5</t>
+  </si>
+  <si>
+    <t>ecoli-0-3-4-7_vs_5-6</t>
+  </si>
+  <si>
+    <t>ecoli-0-3-4_vs_5</t>
+  </si>
+  <si>
+    <t>ecoli-0-4-6_vs_5</t>
+  </si>
+  <si>
+    <t>ecoli-0-6-7_vs_3-5</t>
+  </si>
+  <si>
+    <t>ecoli-0-6-7_vs_5</t>
+  </si>
+  <si>
+    <t>ecoli1</t>
+  </si>
+  <si>
+    <t>ecoli2</t>
+  </si>
+  <si>
+    <t>ecoli3</t>
+  </si>
+  <si>
+    <t>ecoli4</t>
+  </si>
+  <si>
+    <t>eligibility-loan</t>
+  </si>
+  <si>
+    <t>glass-0-1-4-6_vs_2</t>
+  </si>
+  <si>
+    <t>glass-0-1-5_vs_2</t>
+  </si>
+  <si>
+    <t>glass-0-1-6_vs_2</t>
+  </si>
+  <si>
+    <t>glass-0-1-6_vs_5</t>
+  </si>
+  <si>
+    <t>glass-0-4_vs_5</t>
+  </si>
+  <si>
+    <t>glass-0-6_vs_5</t>
+  </si>
+  <si>
+    <t>glass0</t>
+  </si>
+  <si>
+    <t>glass0123vs456</t>
+  </si>
+  <si>
+    <t>glass1</t>
+  </si>
+  <si>
+    <t>glass2</t>
+  </si>
+  <si>
+    <t>glass4</t>
+  </si>
+  <si>
+    <t>glass5</t>
+  </si>
+  <si>
+    <t>glass6</t>
+  </si>
+  <si>
+    <t>haberman</t>
+  </si>
+  <si>
+    <t>leaf</t>
+  </si>
+  <si>
+    <t>led7digit-0-2-4-5-6-7-8-9_vs_1</t>
+  </si>
+  <si>
+    <t>maternal-Risk-lmvsh</t>
+  </si>
+  <si>
+    <t>new-thyroid1</t>
+  </si>
+  <si>
+    <t>oil_spill</t>
+  </si>
+  <si>
+    <t>page-blocks-1-3_vs_4</t>
+  </si>
+  <si>
+    <t>page-blocks1vs2345</t>
+  </si>
+  <si>
+    <t>page-blocks2vs4</t>
+  </si>
+  <si>
+    <t>page-blocks3vs5</t>
+  </si>
+  <si>
+    <t>parkinsons</t>
+  </si>
+  <si>
+    <t>pima-indians-diabetes</t>
+  </si>
+  <si>
+    <t>sampledata1</t>
+  </si>
+  <si>
+    <t>sampledata_new_1</t>
+  </si>
+  <si>
+    <t>sampledata_new_2</t>
+  </si>
+  <si>
+    <t>sampledata_new_3</t>
+  </si>
+  <si>
+    <t>seeds</t>
+  </si>
+  <si>
+    <t>shuttle-4vs5</t>
+  </si>
+  <si>
+    <t>vertebral</t>
+  </si>
+  <si>
+    <t>vowel0</t>
+  </si>
+  <si>
+    <t>wheat1</t>
+  </si>
+  <si>
+    <t>wilt</t>
+  </si>
+  <si>
+    <t>winequality-red-3456vs78</t>
+  </si>
+  <si>
+    <t>wpbc</t>
+  </si>
+  <si>
+    <t>yeast-0-2-5-6_vs_3-7-8-9</t>
+  </si>
+  <si>
+    <t>yeast-0-3-5-9_vs_7-8</t>
+  </si>
+  <si>
+    <t>yeast-0-5-6-7-9_vs_4</t>
+  </si>
+  <si>
+    <t>yeast-1-2-8-9_vs_7</t>
+  </si>
+  <si>
+    <t>yeast-1-4-5-8_vs_7</t>
+  </si>
+  <si>
+    <t>yeast-1_vs_7</t>
+  </si>
+  <si>
+    <t>yeast-2_vs_4</t>
+  </si>
+  <si>
+    <t>yeast-2_vs_8</t>
+  </si>
+  <si>
+    <t>yeast1</t>
+  </si>
+  <si>
+    <t>yeast3</t>
+  </si>
+  <si>
+    <t>yeast4</t>
+  </si>
+  <si>
+    <t>yeast5</t>
+  </si>
+  <si>
     <t>Class1</t>
   </si>
   <si>
@@ -50,603 +272,38 @@
   </si>
   <si>
     <t>label</t>
-  </si>
-  <si>
-    <t>abalone19</t>
-  </si>
-  <si>
-    <t>abalone4–8</t>
-  </si>
-  <si>
-    <t>abalone5–10</t>
-  </si>
-  <si>
-    <t>abalone9-18</t>
-  </si>
-  <si>
-    <t>Breast</t>
-  </si>
-  <si>
-    <t>cleveland-0_vs_4</t>
-  </si>
-  <si>
-    <t>ecoli-0-1-3-7_vs_2-6</t>
-  </si>
-  <si>
-    <t>ecoli-0-1-4-6_vs_5</t>
-  </si>
-  <si>
-    <t>ecoli-0-1-4-7_vs_2-3-5-6</t>
-  </si>
-  <si>
-    <t>ecoli-0-1-4-7_vs_5-6</t>
-  </si>
-  <si>
-    <t>ecoli-0-1_vs_2-3-5</t>
-  </si>
-  <si>
-    <t>ecoli-0-1_vs_5</t>
-  </si>
-  <si>
-    <t>ecoli-0-2-3-4_vs_5</t>
-  </si>
-  <si>
-    <t>ecoli-0-2-6-7_vs_3-5</t>
-  </si>
-  <si>
-    <t>ecoli-0-3-4-6_vs_5</t>
-  </si>
-  <si>
-    <t>ecoli-0-3-4-7_vs_5-6</t>
-  </si>
-  <si>
-    <t>ecoli-0-3-4_vs_5</t>
-  </si>
-  <si>
-    <t>ecoli-0-4-6_vs_5</t>
-  </si>
-  <si>
-    <t>ecoli-0-6-7_vs_3-5</t>
-  </si>
-  <si>
-    <t>ecoli-0-6-7_vs_5</t>
-  </si>
-  <si>
-    <t>ecoli1</t>
-  </si>
-  <si>
-    <t>ecoli2</t>
-  </si>
-  <si>
-    <t>ecoli3</t>
-  </si>
-  <si>
-    <t>ecoli4</t>
-  </si>
-  <si>
-    <t>eligibility-loan</t>
-  </si>
-  <si>
-    <t>glass-0-1-4-6_vs_2</t>
-  </si>
-  <si>
-    <t>glass-0-1-5_vs_2</t>
-  </si>
-  <si>
-    <t>glass-0-1-6_vs_2</t>
-  </si>
-  <si>
-    <t>glass-0-1-6_vs_5</t>
-  </si>
-  <si>
-    <t>glass-0-4_vs_5</t>
-  </si>
-  <si>
-    <t>glass-0-6_vs_5</t>
-  </si>
-  <si>
-    <t>glass0</t>
-  </si>
-  <si>
-    <t>glass0123vs456</t>
-  </si>
-  <si>
-    <t>glass1</t>
-  </si>
-  <si>
-    <t>glass2</t>
-  </si>
-  <si>
-    <t>glass4</t>
-  </si>
-  <si>
-    <t>glass5</t>
-  </si>
-  <si>
-    <t>glass6</t>
-  </si>
-  <si>
-    <t>haberman</t>
-  </si>
-  <si>
-    <t>leaf</t>
-  </si>
-  <si>
-    <t>led7digit-0-2-4-5-6-7-8-9_vs_1</t>
-  </si>
-  <si>
-    <t>Maternal-Risk-lmvsh</t>
-  </si>
-  <si>
-    <t>new-thyroid1</t>
-  </si>
-  <si>
-    <t>oil_spill</t>
-  </si>
-  <si>
-    <t>page-blocks-1-3_vs_4</t>
-  </si>
-  <si>
-    <t>page-blocks1vs2345</t>
-  </si>
-  <si>
-    <t>page-blocks2vs4</t>
-  </si>
-  <si>
-    <t>page-blocks3vs5</t>
-  </si>
-  <si>
-    <t>parkinsons</t>
-  </si>
-  <si>
-    <t>pima-indians-diabetes</t>
-  </si>
-  <si>
-    <t>Sampledata1</t>
-  </si>
-  <si>
-    <t>Sampledata_new_1</t>
-  </si>
-  <si>
-    <t>Sampledata_new_2</t>
-  </si>
-  <si>
-    <t>Sampledata_new_3</t>
-  </si>
-  <si>
-    <t>seeds</t>
-  </si>
-  <si>
-    <t>shuttle-4vs5</t>
-  </si>
-  <si>
-    <t>vertebral</t>
-  </si>
-  <si>
-    <t>vowel0</t>
-  </si>
-  <si>
-    <t>wheat1</t>
-  </si>
-  <si>
-    <t>wilt</t>
-  </si>
-  <si>
-    <t>winequality-red-3456vs78</t>
-  </si>
-  <si>
-    <t>wpbc</t>
-  </si>
-  <si>
-    <t>yeast-0-2-5-6_vs_3-7-8-9</t>
-  </si>
-  <si>
-    <t>yeast-0-3-5-9_vs_7-8</t>
-  </si>
-  <si>
-    <t>yeast-0-5-6-7-9_vs_4</t>
-  </si>
-  <si>
-    <t>yeast-1-2-8-9_vs_7</t>
-  </si>
-  <si>
-    <t>yeast-1-4-5-8_vs_7</t>
-  </si>
-  <si>
-    <t>yeast-1_vs_7</t>
-  </si>
-  <si>
-    <t>yeast-2_vs_4</t>
-  </si>
-  <si>
-    <t>yeast-2_vs_8</t>
-  </si>
-  <si>
-    <t>yeast1</t>
-  </si>
-  <si>
-    <t>yeast3</t>
-  </si>
-  <si>
-    <t>yeast4</t>
-  </si>
-  <si>
-    <t>yeast5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -669,251 +326,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -921,63 +336,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1260,22 +623,17 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="8" width="31.4444444444444" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -1308,10 +666,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -1326,18 +684,18 @@
         <v>8.4</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -1352,18 +710,18 @@
         <v>129.53</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -1375,21 +733,21 @@
         <v>568</v>
       </c>
       <c r="G4">
-        <v>9.96</v>
+        <v>9.960000000000001</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -1404,18 +762,18 @@
         <v>5.51</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -1430,18 +788,18 @@
         <v>16.4</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -1456,18 +814,18 @@
         <v>1.68</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D8">
         <v>13</v>
@@ -1482,18 +840,18 @@
         <v>12.31</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1508,18 +866,18 @@
         <v>39.14</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -1534,18 +892,18 @@
         <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -1560,18 +918,18 @@
         <v>10.59</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D12">
         <v>6</v>
@@ -1586,18 +944,18 @@
         <v>12.28</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -1612,18 +970,18 @@
         <v>9.17</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -1638,18 +996,18 @@
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D15">
         <v>7</v>
@@ -1664,18 +1022,18 @@
         <v>9.1</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -1690,18 +1048,18 @@
         <v>9.18</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -1716,18 +1074,18 @@
         <v>9.25</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D18">
         <v>7</v>
@@ -1739,21 +1097,21 @@
         <v>232</v>
       </c>
       <c r="G18">
-        <v>9.28</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D19">
         <v>7</v>
@@ -1768,18 +1126,18 @@
         <v>9</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -1794,18 +1152,18 @@
         <v>9.15</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D21">
         <v>7</v>
@@ -1820,18 +1178,18 @@
         <v>9.09</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -1846,18 +1204,18 @@
         <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D23">
         <v>7</v>
@@ -1872,18 +1230,18 @@
         <v>3.36</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D24">
         <v>7</v>
@@ -1898,18 +1256,18 @@
         <v>5.46</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D25">
         <v>7</v>
@@ -1924,18 +1282,18 @@
         <v>8.6</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>7</v>
@@ -1950,18 +1308,18 @@
         <v>15.8</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D27">
         <v>11</v>
@@ -1976,18 +1334,18 @@
         <v>2.2</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D28">
         <v>9</v>
@@ -2002,18 +1360,18 @@
         <v>11.06</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D29">
         <v>9</v>
@@ -2025,21 +1383,21 @@
         <v>155</v>
       </c>
       <c r="G29">
-        <v>9.12</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D30">
         <v>9</v>
@@ -2054,18 +1412,18 @@
         <v>10.29</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D31">
         <v>9</v>
@@ -2080,18 +1438,18 @@
         <v>19.44</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D32">
         <v>9</v>
@@ -2103,21 +1461,21 @@
         <v>83</v>
       </c>
       <c r="G32">
-        <v>9.22</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="H32" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D33">
         <v>9</v>
@@ -2132,18 +1490,18 @@
         <v>11</v>
       </c>
       <c r="H33" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D34">
         <v>9</v>
@@ -2158,18 +1516,18 @@
         <v>2.06</v>
       </c>
       <c r="H34" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D35">
         <v>9</v>
@@ -2184,18 +1542,18 @@
         <v>3.2</v>
       </c>
       <c r="H35" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D36">
         <v>9</v>
@@ -2210,18 +1568,18 @@
         <v>2.06</v>
       </c>
       <c r="H36" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D37">
         <v>9</v>
@@ -2236,18 +1594,18 @@
         <v>11.59</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D38">
         <v>9</v>
@@ -2262,18 +1620,18 @@
         <v>15.46</v>
       </c>
       <c r="H38" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D39">
         <v>9</v>
@@ -2288,18 +1646,18 @@
         <v>22.78</v>
       </c>
       <c r="H39" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D40">
         <v>9</v>
@@ -2314,18 +1672,18 @@
         <v>6.38</v>
       </c>
       <c r="H40" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D41">
         <v>3</v>
@@ -2340,18 +1698,18 @@
         <v>2.78</v>
       </c>
       <c r="H41" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D42">
         <v>15</v>
@@ -2366,18 +1724,18 @@
         <v>3.86</v>
       </c>
       <c r="H42" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D43">
         <v>7</v>
@@ -2392,18 +1750,18 @@
         <v>10.97</v>
       </c>
       <c r="H43" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D44">
         <v>6</v>
@@ -2418,18 +1776,18 @@
         <v>2.73</v>
       </c>
       <c r="H44" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D45">
         <v>5</v>
@@ -2444,18 +1802,18 @@
         <v>5.14</v>
       </c>
       <c r="H45" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D46">
         <v>48</v>
@@ -2470,18 +1828,18 @@
         <v>21.85</v>
       </c>
       <c r="H46" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D47">
         <v>10</v>
@@ -2496,18 +1854,18 @@
         <v>15.86</v>
       </c>
       <c r="H47" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D48">
         <v>10</v>
@@ -2522,18 +1880,18 @@
         <v>8.77</v>
       </c>
       <c r="H48" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -2548,18 +1906,18 @@
         <v>3.74</v>
       </c>
       <c r="H49" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D50">
         <v>10</v>
@@ -2574,18 +1932,18 @@
         <v>4.11</v>
       </c>
       <c r="H50" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D51">
         <v>22</v>
@@ -2600,18 +1958,18 @@
         <v>3.06</v>
       </c>
       <c r="H51" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D52">
         <v>8</v>
@@ -2626,18 +1984,18 @@
         <v>1.87</v>
       </c>
       <c r="H52" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -2652,18 +2010,18 @@
         <v>5</v>
       </c>
       <c r="H53" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -2678,18 +2036,18 @@
         <v>5</v>
       </c>
       <c r="H54" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -2704,18 +2062,18 @@
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -2730,18 +2088,18 @@
         <v>2.33</v>
       </c>
       <c r="H56" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D57">
         <v>7</v>
@@ -2756,18 +2114,18 @@
         <v>2</v>
       </c>
       <c r="H57" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D58">
         <v>9</v>
@@ -2782,18 +2140,18 @@
         <v>2.66</v>
       </c>
       <c r="H58" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D59">
         <v>6</v>
@@ -2808,18 +2166,18 @@
         <v>2.1</v>
       </c>
       <c r="H59" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D60">
         <v>13</v>
@@ -2834,18 +2192,18 @@
         <v>9.98</v>
       </c>
       <c r="H60" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D61">
         <v>7</v>
@@ -2860,18 +2218,18 @@
         <v>2</v>
       </c>
       <c r="H61" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D62">
         <v>5</v>
@@ -2886,18 +2244,18 @@
         <v>57.64</v>
       </c>
       <c r="H62" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D63">
         <v>11</v>
@@ -2912,18 +2270,18 @@
         <v>6.37</v>
       </c>
       <c r="H63" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D64">
         <v>31</v>
@@ -2938,18 +2296,18 @@
         <v>1.68</v>
       </c>
       <c r="H64" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D65">
         <v>8</v>
@@ -2961,21 +2319,21 @@
         <v>905</v>
       </c>
       <c r="G65">
-        <v>9.14</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="H65" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D66">
         <v>8</v>
@@ -2987,21 +2345,21 @@
         <v>456</v>
       </c>
       <c r="G66">
-        <v>9.12</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="H66" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D67">
         <v>8</v>
@@ -3016,18 +2374,18 @@
         <v>9.35</v>
       </c>
       <c r="H67" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D68">
         <v>8</v>
@@ -3042,18 +2400,18 @@
         <v>30.57</v>
       </c>
       <c r="H68" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D69">
         <v>8</v>
@@ -3068,18 +2426,18 @@
         <v>22.1</v>
       </c>
       <c r="H69" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D70">
         <v>7</v>
@@ -3094,18 +2452,18 @@
         <v>14.3</v>
       </c>
       <c r="H70" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D71">
         <v>8</v>
@@ -3120,18 +2478,18 @@
         <v>9.08</v>
       </c>
       <c r="H71" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D72">
         <v>8</v>
@@ -3146,18 +2504,18 @@
         <v>23.1</v>
       </c>
       <c r="H72" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D73">
         <v>8</v>
@@ -3172,18 +2530,18 @@
         <v>2.46</v>
       </c>
       <c r="H73" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D74">
         <v>8</v>
@@ -3198,18 +2556,18 @@
         <v>8.1</v>
       </c>
       <c r="H74" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D75">
         <v>8</v>
@@ -3224,18 +2582,18 @@
         <v>28.1</v>
       </c>
       <c r="H75" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D76">
         <v>8</v>
@@ -3250,11 +2608,10 @@
         <v>32.73</v>
       </c>
       <c r="H76" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
split datasets and create new read fold function
</commit_message>
<xml_diff>
--- a/Datasets/dataset_description.xlsx
+++ b/Datasets/dataset_description.xlsx
@@ -451,7 +451,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +461,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,12 +599,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,10 +784,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -790,16 +796,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -811,10 +817,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -835,28 +841,28 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -865,22 +871,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -889,43 +889,51 @@
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1275,7 +1283,7 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A7" sqref="$A3:$XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1371,7 +1379,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
@@ -1400,7 +1408,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
@@ -1429,7 +1437,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
@@ -1574,7 +1582,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
@@ -1835,7 +1843,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
@@ -1922,7 +1930,7 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B23" t="s">
@@ -2183,7 +2191,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B32" t="s">

</xml_diff>